<commit_message>
add exe file and final file
</commit_message>
<xml_diff>
--- a/sources_file/source.xlsx
+++ b/sources_file/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\BAST_Creator\sources_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E265E3F-D4F4-4BD2-AD9D-7CFE247DF79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C92D2-FA22-4452-A53E-1CE08AB0876E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D234A5E-3EAB-42EF-91DF-BBB15EF7C46F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Project ID</t>
   </si>
@@ -48,106 +48,58 @@
     <t>Alamat</t>
   </si>
   <si>
+    <t>Mitra</t>
+  </si>
+  <si>
+    <t>Nilai Kontrak</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>SOW</t>
+  </si>
+  <si>
+    <t>Tanggal PKS</t>
+  </si>
+  <si>
+    <t>Tanggal PO</t>
+  </si>
+  <si>
+    <t>Tipe Tower</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Jabatan GM</t>
+  </si>
+  <si>
+    <t>Nama GM</t>
+  </si>
+  <si>
+    <t>Jabatan Manager Asset</t>
+  </si>
+  <si>
+    <t>Nama Manager Asset</t>
+  </si>
+  <si>
+    <t>Nama Asman Asset</t>
+  </si>
+  <si>
+    <t>Jabatan Asman Asset</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jangka Waktu Kerja</t>
+  </si>
+  <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>Mitra</t>
-  </si>
-  <si>
-    <t>Nilai Kontrak</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Lat</t>
-  </si>
-  <si>
-    <t>SOW</t>
-  </si>
-  <si>
-    <t>Tanggal PKS</t>
-  </si>
-  <si>
-    <t>Tanggal PO</t>
-  </si>
-  <si>
-    <t>Tipe Tower</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Jabatan GM</t>
-  </si>
-  <si>
-    <t>Nama GM</t>
-  </si>
-  <si>
-    <t>Jabatan Manager Asset</t>
-  </si>
-  <si>
-    <t>Nama Manager Asset</t>
-  </si>
-  <si>
-    <t>Nama Asman Asset</t>
-  </si>
-  <si>
-    <t>Jabatan Asman Asset</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>091/PM2/A1000000/III/24</t>
-  </si>
-  <si>
-    <t>SST</t>
-  </si>
-  <si>
-    <t>PT ATMAJAYA ARTHA PERKASA</t>
-  </si>
-  <si>
-    <t>GM Area IV Pamasuka</t>
-  </si>
-  <si>
-    <t>Mgr. Asset Reg Sulawesi &amp; Malut</t>
-  </si>
-  <si>
-    <t>Asman Asset Sulawesi &amp; Malut</t>
-  </si>
-  <si>
-    <t>Rudi Albert</t>
-  </si>
-  <si>
-    <t>Muhammad Ershad</t>
-  </si>
-  <si>
-    <t>Hanafi Nur Arifin</t>
-  </si>
-  <si>
-    <t>Jangka Waktu Kerja</t>
-  </si>
-  <si>
-    <t>Survey Collocation</t>
-  </si>
-  <si>
-    <t>BANGUN_MERIAH_MT</t>
-  </si>
-  <si>
-    <t>PMS1-01-182</t>
-  </si>
-  <si>
-    <t>70 (SM)</t>
-  </si>
-  <si>
-    <t>Huta Tinggir, Desa Tano Tinggir, Kec. Purba, Kab. Simalungun, Provinsi. Sumatera Utara</t>
-  </si>
-  <si>
-    <t>01. SUMBAGUT</t>
-  </si>
-  <si>
-    <t>24IS11C0061</t>
   </si>
 </sst>
 </file>
@@ -688,7 +640,7 @@
   <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +674,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -740,139 +692,89 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="22">
-        <v>45359</v>
-      </c>
-      <c r="H2" s="23">
-        <v>4100118118</v>
-      </c>
-      <c r="I2" s="22">
-        <v>45644</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="7">
-        <v>98.61497</v>
-      </c>
-      <c r="N2" s="7">
-        <v>2.89899</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="11">
-        <v>10575000</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="9">
-        <v>7</v>
-      </c>
+      <c r="A2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>

</xml_diff>